<commit_message>
added Reuse Existing Terms metric + test
</commit_message>
<xml_diff>
--- a/lod-qualitymetrics/lod-qualitymetrics-representation/src/test/resources/metric_values.xlsx
+++ b/lod-qualitymetrics/lod-qualitymetrics-representation/src/test/resources/metric_values.xlsx
@@ -4,11 +4,12 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25203"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14720" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14720" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Undefined Classes and Props" sheetId="1" r:id="rId1"/>
     <sheet name="Short URI" sheetId="2" r:id="rId2"/>
+    <sheet name="Reused Terms" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -20,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="690" uniqueCount="689">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="717" uniqueCount="711">
   <si>
     <t>eis:CommunityProject</t>
   </si>
@@ -2087,6 +2088,72 @@
   </si>
   <si>
     <t>Short URI</t>
+  </si>
+  <si>
+    <t>Classes</t>
+  </si>
+  <si>
+    <t>swrc:Conference</t>
+  </si>
+  <si>
+    <t>geonames:SpatialThing</t>
+  </si>
+  <si>
+    <t>Properties</t>
+  </si>
+  <si>
+    <t>swrc:startDate</t>
+  </si>
+  <si>
+    <t>swrc:description</t>
+  </si>
+  <si>
+    <t>dcterms:spatial</t>
+  </si>
+  <si>
+    <t>swrc:eventTitle</t>
+  </si>
+  <si>
+    <t>swrc:location</t>
+  </si>
+  <si>
+    <t>geonames:name</t>
+  </si>
+  <si>
+    <t>geo:long</t>
+  </si>
+  <si>
+    <t>geonames:P</t>
+  </si>
+  <si>
+    <t>geo:lat</t>
+  </si>
+  <si>
+    <t>geonames:countryName</t>
+  </si>
+  <si>
+    <t>wgs84_pos</t>
+  </si>
+  <si>
+    <t>geonames</t>
+  </si>
+  <si>
+    <t>swrc</t>
+  </si>
+  <si>
+    <t>swc</t>
+  </si>
+  <si>
+    <t>Others (Top)</t>
+  </si>
+  <si>
+    <t>Total</t>
+  </si>
+  <si>
+    <t>Total Reused Terms</t>
+  </si>
+  <si>
+    <t>Total Unique Terms</t>
   </si>
 </sst>
 </file>
@@ -2172,147 +2239,7 @@
     <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="17">
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="3">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -3886,12 +3813,12 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B1:B35 B38:B40">
-    <cfRule type="cellIs" dxfId="3" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="2" operator="equal">
       <formula>FALSE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B40:B147">
-    <cfRule type="cellIs" dxfId="2" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
       <formula>FALSE</formula>
     </cfRule>
   </conditionalFormatting>
@@ -3909,7 +3836,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E535"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
@@ -8572,7 +8499,7 @@
         <v>666</v>
       </c>
       <c r="B515" t="b">
-        <f t="shared" ref="B515:B547" si="8">IF(OR(ISNUMBER(FIND("?",A515)),LEN(A515) &gt; 80), FALSE, TRUE)</f>
+        <f t="shared" ref="B515:B535" si="8">IF(OR(ISNUMBER(FIND("?",A515)),LEN(A515) &gt; 80), FALSE, TRUE)</f>
         <v>1</v>
       </c>
     </row>
@@ -8758,7 +8685,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B1:B1048576">
-    <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="0" priority="2" operator="equal">
       <formula>FALSE</formula>
     </cfRule>
   </conditionalFormatting>
@@ -8769,4 +8696,229 @@
     </ext>
   </extLst>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:I22"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F12" sqref="F12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="1" max="1" width="28.83203125" customWidth="1"/>
+    <col min="6" max="6" width="11.5" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="17.33203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9">
+      <c r="B1" t="s">
+        <v>703</v>
+      </c>
+      <c r="C1" t="s">
+        <v>704</v>
+      </c>
+      <c r="D1" t="s">
+        <v>705</v>
+      </c>
+      <c r="E1" t="s">
+        <v>706</v>
+      </c>
+      <c r="F1" t="s">
+        <v>707</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9">
+      <c r="A2" s="1" t="s">
+        <v>689</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9">
+      <c r="A3" t="s">
+        <v>690</v>
+      </c>
+      <c r="D3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9">
+      <c r="A4" t="s">
+        <v>691</v>
+      </c>
+      <c r="C4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9">
+      <c r="A6" s="1" t="s">
+        <v>692</v>
+      </c>
+      <c r="H6" t="s">
+        <v>709</v>
+      </c>
+      <c r="I6">
+        <f>SUM(B22:F22)</f>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9">
+      <c r="A7" t="s">
+        <v>31</v>
+      </c>
+      <c r="F7">
+        <v>1</v>
+      </c>
+      <c r="H7" t="s">
+        <v>710</v>
+      </c>
+      <c r="I7">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9">
+      <c r="A8" t="s">
+        <v>693</v>
+      </c>
+      <c r="D8">
+        <v>0</v>
+      </c>
+      <c r="H8" t="s">
+        <v>150</v>
+      </c>
+      <c r="I8">
+        <f>I6/I7</f>
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9">
+      <c r="A9" t="s">
+        <v>694</v>
+      </c>
+      <c r="D9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9">
+      <c r="A10" t="s">
+        <v>40</v>
+      </c>
+      <c r="F10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9">
+      <c r="A11" t="s">
+        <v>695</v>
+      </c>
+      <c r="F11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9">
+      <c r="A12" t="s">
+        <v>696</v>
+      </c>
+      <c r="D12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9">
+      <c r="A13" t="s">
+        <v>697</v>
+      </c>
+      <c r="D13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9">
+      <c r="A14" t="s">
+        <v>97</v>
+      </c>
+      <c r="F14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9">
+      <c r="A15" t="s">
+        <v>45</v>
+      </c>
+      <c r="F15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9">
+      <c r="A16" t="s">
+        <v>698</v>
+      </c>
+      <c r="C16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6">
+      <c r="A17" t="s">
+        <v>699</v>
+      </c>
+      <c r="B17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6">
+      <c r="A18" t="s">
+        <v>700</v>
+      </c>
+      <c r="C18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6">
+      <c r="A19" t="s">
+        <v>701</v>
+      </c>
+      <c r="B19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6">
+      <c r="A20" t="s">
+        <v>702</v>
+      </c>
+      <c r="C20">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6">
+      <c r="A22" s="1" t="s">
+        <v>708</v>
+      </c>
+      <c r="B22">
+        <f>COUNTIF(B2:B20,1)</f>
+        <v>2</v>
+      </c>
+      <c r="C22">
+        <f t="shared" ref="C22:F22" si="0">COUNTIF(C2:C20,1)</f>
+        <v>2</v>
+      </c>
+      <c r="D22">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="E22">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F22">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
 </file>
</xml_diff>